<commit_message>
Return to work on project commit
</commit_message>
<xml_diff>
--- a/pub_quiz_app/_documentation/Presentation Excel Datastructure.xlsx
+++ b/pub_quiz_app/_documentation/Presentation Excel Datastructure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/codeclan/codeclan_work/solo_project/pub_quiz_app/_documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3DED69-056F-154C-A5D4-8082B3362F1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF82E6DB-7FC2-E043-943A-3F176E099D5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{C893E412-18C1-4642-998B-F82C98FD3B95}"/>
   </bookViews>
@@ -526,7 +526,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="81">
+  <borders count="84">
     <border>
       <left/>
       <right/>
@@ -1536,11 +1536,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="dashed">
+        <color rgb="FF00B050"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dashed">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF00B050"/>
+      </right>
+      <top style="dashed">
+        <color rgb="FF00B050"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1843,6 +1874,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2166,7 +2209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EEA5900-EB13-8645-960A-A74230A52A32}">
   <dimension ref="A1:BQ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="AX27" sqref="AX26:AZ27"/>
     </sheetView>
   </sheetViews>
@@ -3888,9 +3931,9 @@
       <c r="AU25" s="88"/>
       <c r="AV25" s="86"/>
       <c r="AW25" s="87"/>
-      <c r="AX25" s="88"/>
-      <c r="AY25" s="86"/>
-      <c r="AZ25" s="89"/>
+      <c r="AX25" s="102"/>
+      <c r="AY25" s="103"/>
+      <c r="AZ25" s="104"/>
       <c r="BA25" s="41"/>
       <c r="BB25" s="42"/>
       <c r="BC25" s="42"/>
@@ -3965,11 +4008,11 @@
       <c r="AT26" s="42"/>
       <c r="AU26" s="42"/>
       <c r="AV26" s="42"/>
-      <c r="AW26" s="42"/>
-      <c r="AX26" s="42"/>
-      <c r="AY26" s="42"/>
-      <c r="AZ26" s="43"/>
-      <c r="BA26" s="41"/>
+      <c r="AW26" s="88"/>
+      <c r="AX26" s="105"/>
+      <c r="AY26" s="105"/>
+      <c r="AZ26" s="105"/>
+      <c r="BA26" s="87"/>
       <c r="BB26" s="42"/>
       <c r="BC26" s="42"/>
       <c r="BD26" s="42"/>
@@ -4043,11 +4086,11 @@
       <c r="AT27" s="42"/>
       <c r="AU27" s="42"/>
       <c r="AV27" s="42"/>
-      <c r="AW27" s="42"/>
-      <c r="AX27" s="42"/>
-      <c r="AY27" s="42"/>
-      <c r="AZ27" s="43"/>
-      <c r="BA27" s="41"/>
+      <c r="AW27" s="88"/>
+      <c r="AX27" s="105"/>
+      <c r="AY27" s="105"/>
+      <c r="AZ27" s="105"/>
+      <c r="BA27" s="87"/>
       <c r="BB27" s="42"/>
       <c r="BC27" s="42"/>
       <c r="BD27" s="42"/>
@@ -4122,9 +4165,9 @@
       <c r="AU28" s="42"/>
       <c r="AV28" s="42"/>
       <c r="AW28" s="42"/>
-      <c r="AX28" s="42"/>
-      <c r="AY28" s="42"/>
-      <c r="AZ28" s="43"/>
+      <c r="AX28" s="39"/>
+      <c r="AY28" s="39"/>
+      <c r="AZ28" s="40"/>
       <c r="BA28" s="41"/>
       <c r="BB28" s="42"/>
       <c r="BC28" s="42"/>
@@ -4363,6 +4406,10 @@
       <c r="BF32" s="64"/>
       <c r="BG32" s="64"/>
       <c r="BH32" s="65"/>
+      <c r="BI32" s="69"/>
+      <c r="BK32" s="64"/>
+      <c r="BM32" s="64"/>
+      <c r="BO32" s="64"/>
     </row>
     <row r="33" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>